<commit_message>
edit protocol documentadded value column in create room result protocol
</commit_message>
<xml_diff>
--- a/doc/프로토콜_명세.xlsx
+++ b/doc/프로토콜_명세.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\배용호\Documents\GitHub\NoDoubt\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ide\eclipse\NoDoubt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3504" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3504"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,10 +385,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Room : Room Object</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MasterID : String, RoomName : String, 
 Password: String</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -698,13 +694,17 @@
   </si>
   <si>
     <t>완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value: Boolean, Room : Room Object</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1123,10 +1123,10 @@
         <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1149,10 +1149,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1175,67 +1175,67 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -1253,7 +1253,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1290,13 +1290,13 @@
         <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1313,13 +1313,13 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1342,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1359,13 +1359,13 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1376,19 +1376,19 @@
         <v>64</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1411,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1434,7 +1434,7 @@
         <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1497,7 +1497,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1520,7 +1520,7 @@
         <v>45</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1543,7 +1543,7 @@
         <v>49</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1633,141 +1633,141 @@
         <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1775,16 +1775,16 @@
     </row>
     <row r="8" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="1"/>
@@ -1793,93 +1793,93 @@
     </row>
     <row r="9" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="E9" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">

</xml_diff>